<commit_message>
mass analysis for the lower injector
</commit_message>
<xml_diff>
--- a/analysis/mass_analysis_bilbo/BC02.xlsx
+++ b/analysis/mass_analysis_bilbo/BC02.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D290"/>
+  <dimension ref="A1:D206"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,10 +477,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01548509822117137</v>
+        <v>0.01547</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01548509822117137</v>
+        <v>0.01547</v>
       </c>
     </row>
     <row r="4">
@@ -491,10 +491,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03370271603927411</v>
+        <v>0.03367</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03370271603927411</v>
+        <v>0.03367</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.01162403396342168</v>
+        <v>0.01434151890507272</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04029734758769313</v>
+        <v>0.03752848109492728</v>
       </c>
       <c r="D5" t="n">
-        <v>0.05192138155111481</v>
+        <v>0.05187</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.03376024183404012</v>
+        <v>0.04127349191751366</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03631564396908004</v>
+        <v>0.02879650808248633</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07007588580312016</v>
+        <v>0.07006999999999999</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.03856872619209623</v>
+        <v>0.04745553793107396</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04972427237454024</v>
+        <v>0.04081446206892604</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08829299856663647</v>
+        <v>0.08827</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.06034936334897398</v>
+        <v>0.07405613415974621</v>
       </c>
       <c r="C8" t="n">
-        <v>0.04616127196827887</v>
+        <v>0.03241386584025378</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1065106353172529</v>
+        <v>0.10647</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.07114450015972135</v>
+        <v>0.08793333354685684</v>
       </c>
       <c r="C9" t="n">
-        <v>0.05357800112540284</v>
+        <v>0.03673666645314316</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1247225012851242</v>
+        <v>0.12467</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.08016663681270554</v>
+        <v>0.09928085320489323</v>
       </c>
       <c r="C10" t="n">
-        <v>0.06270926657628596</v>
+        <v>0.04358914679510677</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1428759033889915</v>
+        <v>0.14287</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.08397720041110611</v>
+        <v>0.1043893310726796</v>
       </c>
       <c r="C11" t="n">
-        <v>0.07712339633994243</v>
+        <v>0.05668066892732042</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1611005967510485</v>
+        <v>0.16107</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.09332409584072514</v>
+        <v>0.1165401525609081</v>
       </c>
       <c r="C12" t="n">
-        <v>0.08599003893527839</v>
+        <v>0.06272984743909191</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1793141347760035</v>
+        <v>0.17927</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.09790370151333157</v>
+        <v>0.1219955081823504</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09962226273205095</v>
+        <v>0.07547449181764959</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1975259642453825</v>
+        <v>0.19747</v>
       </c>
     </row>
     <row r="14">
@@ -628,13 +628,13 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.1064868689971232</v>
+        <v>0.1326086141474256</v>
       </c>
       <c r="C14" t="n">
-        <v>0.1091930324017933</v>
+        <v>0.08306138585257439</v>
       </c>
       <c r="D14" t="n">
-        <v>0.2156799013989165</v>
+        <v>0.21567</v>
       </c>
     </row>
     <row r="15">
@@ -642,13 +642,13 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.1144202220069696</v>
+        <v>0.1420806330425586</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1194878726628102</v>
+        <v>0.09178936695744142</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2339080946697798</v>
+        <v>0.23387</v>
       </c>
     </row>
     <row r="16">
@@ -656,13 +656,13 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.1152673281623578</v>
+        <v>0.1430848504189106</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1276376725980946</v>
+        <v>0.09794381624775603</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2429050007604524</v>
+        <v>0.2410286666666667</v>
       </c>
     </row>
     <row r="17">
@@ -670,13 +670,13 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.115893556706128</v>
+        <v>0.1439588359627547</v>
       </c>
       <c r="C17" t="n">
-        <v>0.1434075091424696</v>
+        <v>0.113449830703912</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2593010658485976</v>
+        <v>0.2574086666666667</v>
       </c>
     </row>
     <row r="18">
@@ -684,13 +684,13 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1159231124626202</v>
+        <v>0.1440340433846438</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1616054500782003</v>
+        <v>0.1315746232820228</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2775285625408205</v>
+        <v>0.2756086666666667</v>
       </c>
     </row>
     <row r="19">
@@ -698,13 +698,13 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1175958972363537</v>
+        <v>0.1463686383903795</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1780967011885215</v>
+        <v>0.1474400282762871</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2956925984248752</v>
+        <v>0.2938086666666667</v>
       </c>
     </row>
     <row r="20">
@@ -712,13 +712,13 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.1134043425840337</v>
+        <v>0.1410140126150159</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2005050643389419</v>
+        <v>0.1709946540516507</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3139094069229756</v>
+        <v>0.3120086666666667</v>
       </c>
     </row>
     <row r="21">
@@ -726,13 +726,13 @@
         <v>95</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1150459852168924</v>
+        <v>0.143126758298222</v>
       </c>
       <c r="C21" t="n">
-        <v>0.2170761655316625</v>
+        <v>0.1870819083684447</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3321221507485549</v>
+        <v>0.3302086666666667</v>
       </c>
     </row>
     <row r="22">
@@ -740,13 +740,13 @@
         <v>100</v>
       </c>
       <c r="B22" t="n">
-        <v>0.1154858503448511</v>
+        <v>0.1436119299264478</v>
       </c>
       <c r="C22" t="n">
-        <v>0.2348569197937679</v>
+        <v>0.2047967367402189</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3503427701386189</v>
+        <v>0.3484086666666667</v>
       </c>
     </row>
     <row r="23">
@@ -754,13 +754,13 @@
         <v>105</v>
       </c>
       <c r="B23" t="n">
-        <v>0.1100031362805334</v>
+        <v>0.1368580827748954</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2584946213184832</v>
+        <v>0.2297505838917713</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3684977575990165</v>
+        <v>0.3666086666666667</v>
       </c>
     </row>
     <row r="24">
@@ -768,13 +768,13 @@
         <v>110</v>
       </c>
       <c r="B24" t="n">
-        <v>0.11835648100373</v>
+        <v>0.147317482153167</v>
       </c>
       <c r="C24" t="n">
-        <v>0.2683613975104647</v>
+        <v>0.2374911845134997</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3867178785141947</v>
+        <v>0.3848086666666667</v>
       </c>
     </row>
     <row r="25">
@@ -782,13 +782,13 @@
         <v>115</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1226409180816928</v>
+        <v>0.1525529061861639</v>
       </c>
       <c r="C25" t="n">
-        <v>0.2822958298477635</v>
+        <v>0.2504557604805028</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4049367479294563</v>
+        <v>0.4030086666666667</v>
       </c>
     </row>
     <row r="26">
@@ -796,13 +796,13 @@
         <v>120</v>
       </c>
       <c r="B26" t="n">
-        <v>0.1271249342298437</v>
+        <v>0.158184300048046</v>
       </c>
       <c r="C26" t="n">
-        <v>0.2959677912728611</v>
+        <v>0.2630243666186206</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4230927255027048</v>
+        <v>0.4212086666666667</v>
       </c>
     </row>
     <row r="27">
@@ -810,13 +810,13 @@
         <v>125</v>
       </c>
       <c r="B27" t="n">
-        <v>0.1353519462626666</v>
+        <v>0.1679725866677268</v>
       </c>
       <c r="C27" t="n">
-        <v>0.3059604943184213</v>
+        <v>0.2714360799989398</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4413124405810879</v>
+        <v>0.4394086666666667</v>
       </c>
     </row>
     <row r="28">
@@ -824,13 +824,13 @@
         <v>130</v>
       </c>
       <c r="B28" t="n">
-        <v>0.1394167548053162</v>
+        <v>0.1729101524482979</v>
       </c>
       <c r="C28" t="n">
-        <v>0.3201077794388685</v>
+        <v>0.2846985142183688</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4595245342441847</v>
+        <v>0.4576086666666667</v>
       </c>
     </row>
     <row r="29">
@@ -838,13 +838,13 @@
         <v>135</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1458462039323133</v>
+        <v>0.1808079157038595</v>
       </c>
       <c r="C29" t="n">
-        <v>0.3318987865547389</v>
+        <v>0.2950007509628071</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4777449904870523</v>
+        <v>0.4758086666666667</v>
       </c>
     </row>
     <row r="30">
@@ -852,13 +852,13 @@
         <v>140</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1458665401799824</v>
+        <v>0.18078298798913</v>
       </c>
       <c r="C30" t="n">
-        <v>0.3500380386955873</v>
+        <v>0.3132256786775366</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4959045788755697</v>
+        <v>0.4940086666666667</v>
       </c>
     </row>
     <row r="31">
@@ -866,13 +866,13 @@
         <v>145</v>
       </c>
       <c r="B31" t="n">
-        <v>0.1497674830623586</v>
+        <v>0.1856192985916326</v>
       </c>
       <c r="C31" t="n">
-        <v>0.3637607414391305</v>
+        <v>0.3260130347417006</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5135282245014892</v>
+        <v>0.5116323333333332</v>
       </c>
     </row>
     <row r="32">
@@ -880,13 +880,13 @@
         <v>150</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1491195000074178</v>
+        <v>0.1847638085138917</v>
       </c>
       <c r="C32" t="n">
-        <v>0.3681186275868765</v>
+        <v>0.3305995248194417</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="33">
@@ -894,13 +894,13 @@
         <v>155</v>
       </c>
       <c r="B33" t="n">
-        <v>0.146821442029146</v>
+        <v>0.181934132568961</v>
       </c>
       <c r="C33" t="n">
-        <v>0.3704166855651483</v>
+        <v>0.3334292007643723</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="34">
@@ -908,13 +908,13 @@
         <v>160</v>
       </c>
       <c r="B34" t="n">
-        <v>0.1443576339034015</v>
+        <v>0.1789504834453317</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3728804936908928</v>
+        <v>0.3364128498880016</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="35">
@@ -922,13 +922,13 @@
         <v>165</v>
       </c>
       <c r="B35" t="n">
-        <v>0.1373559682362605</v>
+        <v>0.1703185954667518</v>
       </c>
       <c r="C35" t="n">
-        <v>0.3798821593580338</v>
+        <v>0.3450447378665815</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="36">
@@ -936,13 +936,13 @@
         <v>170</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1354956131911771</v>
+        <v>0.1679388679686967</v>
       </c>
       <c r="C36" t="n">
-        <v>0.3817425144031172</v>
+        <v>0.3474244653646366</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="37">
@@ -950,13 +950,13 @@
         <v>175</v>
       </c>
       <c r="B37" t="n">
-        <v>0.1337081696751002</v>
+        <v>0.1657953208598814</v>
       </c>
       <c r="C37" t="n">
-        <v>0.3835299579191941</v>
+        <v>0.3495680124734519</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="38">
@@ -964,13 +964,13 @@
         <v>180</v>
       </c>
       <c r="B38" t="n">
-        <v>0.1303151956774729</v>
+        <v>0.1615814854591243</v>
       </c>
       <c r="C38" t="n">
-        <v>0.3869229319168214</v>
+        <v>0.353781847874209</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="39">
@@ -978,13 +978,13 @@
         <v>185</v>
       </c>
       <c r="B39" t="n">
-        <v>0.1315479458916307</v>
+        <v>0.1631049054565533</v>
       </c>
       <c r="C39" t="n">
-        <v>0.3856901817026637</v>
+        <v>0.35225842787678</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="40">
@@ -992,13 +992,13 @@
         <v>190</v>
       </c>
       <c r="B40" t="n">
-        <v>0.1277965438801999</v>
+        <v>0.1584960721057116</v>
       </c>
       <c r="C40" t="n">
-        <v>0.3894415837140944</v>
+        <v>0.3568672612276217</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="41">
@@ -1006,13 +1006,13 @@
         <v>195</v>
       </c>
       <c r="B41" t="n">
-        <v>0.1270325972947129</v>
+        <v>0.1575269011522238</v>
       </c>
       <c r="C41" t="n">
-        <v>0.3902055302995814</v>
+        <v>0.3578364321811094</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="42">
@@ -1020,13 +1020,13 @@
         <v>200</v>
       </c>
       <c r="B42" t="n">
-        <v>0.1253396218540546</v>
+        <v>0.1554981979584279</v>
       </c>
       <c r="C42" t="n">
-        <v>0.3918985057402397</v>
+        <v>0.3598651353749054</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="43">
@@ -1034,13 +1034,13 @@
         <v>205</v>
       </c>
       <c r="B43" t="n">
-        <v>0.1241103227953058</v>
+        <v>0.1539522890419175</v>
       </c>
       <c r="C43" t="n">
-        <v>0.3931278047989885</v>
+        <v>0.3614110442914157</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="44">
@@ -1048,13 +1048,13 @@
         <v>210</v>
       </c>
       <c r="B44" t="n">
-        <v>0.1207738166470943</v>
+        <v>0.1497839703919197</v>
       </c>
       <c r="C44" t="n">
-        <v>0.3964643109472</v>
+        <v>0.3655793629414136</v>
       </c>
       <c r="D44" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="45">
@@ -1062,13 +1062,13 @@
         <v>215</v>
       </c>
       <c r="B45" t="n">
-        <v>0.1183307088531136</v>
+        <v>0.1467855440410842</v>
       </c>
       <c r="C45" t="n">
-        <v>0.3989074187411807</v>
+        <v>0.3685777892922491</v>
       </c>
       <c r="D45" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="46">
@@ -1076,13 +1076,13 @@
         <v>220</v>
       </c>
       <c r="B46" t="n">
-        <v>0.1166081424108227</v>
+        <v>0.1446662736955664</v>
       </c>
       <c r="C46" t="n">
-        <v>0.4006299851834716</v>
+        <v>0.3706970596377669</v>
       </c>
       <c r="D46" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="47">
@@ -1090,13 +1090,13 @@
         <v>225</v>
       </c>
       <c r="B47" t="n">
-        <v>0.1139422293893799</v>
+        <v>0.1413781207951708</v>
       </c>
       <c r="C47" t="n">
-        <v>0.4032958982049145</v>
+        <v>0.3739852125381624</v>
       </c>
       <c r="D47" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="48">
@@ -1104,13 +1104,13 @@
         <v>230</v>
       </c>
       <c r="B48" t="n">
-        <v>0.1119626262214246</v>
+        <v>0.1389130407394177</v>
       </c>
       <c r="C48" t="n">
-        <v>0.4052755013728698</v>
+        <v>0.3764502925939156</v>
       </c>
       <c r="D48" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="49">
@@ -1118,13 +1118,13 @@
         <v>235</v>
       </c>
       <c r="B49" t="n">
-        <v>0.1113463787196682</v>
+        <v>0.1381460263447066</v>
       </c>
       <c r="C49" t="n">
-        <v>0.4058917488746261</v>
+        <v>0.3772173069886267</v>
       </c>
       <c r="D49" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="50">
@@ -1132,13 +1132,13 @@
         <v>240</v>
       </c>
       <c r="B50" t="n">
-        <v>0.1097396213900055</v>
+        <v>0.136191812843402</v>
       </c>
       <c r="C50" t="n">
-        <v>0.4074985062042888</v>
+        <v>0.3791715204899313</v>
       </c>
       <c r="D50" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="51">
@@ -1146,13 +1146,13 @@
         <v>245</v>
       </c>
       <c r="B51" t="n">
-        <v>0.1089921471227439</v>
+        <v>0.1352753487708378</v>
       </c>
       <c r="C51" t="n">
-        <v>0.4082459804715504</v>
+        <v>0.3800879845624955</v>
       </c>
       <c r="D51" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="52">
@@ -1160,13 +1160,13 @@
         <v>250</v>
       </c>
       <c r="B52" t="n">
-        <v>0.1089833085966088</v>
+        <v>0.1352453659119549</v>
       </c>
       <c r="C52" t="n">
-        <v>0.4082548189976855</v>
+        <v>0.3801179674213784</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="53">
@@ -1174,13 +1174,13 @@
         <v>255</v>
       </c>
       <c r="B53" t="n">
-        <v>0.1071110355216525</v>
+        <v>0.1329547949918564</v>
       </c>
       <c r="C53" t="n">
-        <v>0.4101270920726419</v>
+        <v>0.3824085383414769</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="54">
@@ -1188,13 +1188,13 @@
         <v>260</v>
       </c>
       <c r="B54" t="n">
-        <v>0.106682274795511</v>
+        <v>0.1324203358941621</v>
       </c>
       <c r="C54" t="n">
-        <v>0.4105558527987834</v>
+        <v>0.3829429974391713</v>
       </c>
       <c r="D54" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="55">
@@ -1202,13 +1202,13 @@
         <v>265</v>
       </c>
       <c r="B55" t="n">
-        <v>0.10490974612738</v>
+        <v>0.1302560123728722</v>
       </c>
       <c r="C55" t="n">
-        <v>0.4123283814669143</v>
+        <v>0.3851073209604611</v>
       </c>
       <c r="D55" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="56">
@@ -1216,13 +1216,13 @@
         <v>270</v>
       </c>
       <c r="B56" t="n">
-        <v>0.1031546275390638</v>
+        <v>0.1280937871075917</v>
       </c>
       <c r="C56" t="n">
-        <v>0.4140835000552305</v>
+        <v>0.3872695462257416</v>
       </c>
       <c r="D56" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="57">
@@ -1230,13 +1230,13 @@
         <v>275</v>
       </c>
       <c r="B57" t="n">
-        <v>0.09839823844049958</v>
+        <v>0.1222593363424883</v>
       </c>
       <c r="C57" t="n">
-        <v>0.4188398891537948</v>
+        <v>0.393103996990845</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="58">
@@ -1244,13 +1244,13 @@
         <v>280</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0919222574554818</v>
+        <v>0.114367329973414</v>
       </c>
       <c r="C58" t="n">
-        <v>0.4253158701388126</v>
+        <v>0.4009960033599193</v>
       </c>
       <c r="D58" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="59">
@@ -1258,13 +1258,13 @@
         <v>285</v>
       </c>
       <c r="B59" t="n">
-        <v>0.09131422066933761</v>
+        <v>0.1135889598364946</v>
       </c>
       <c r="C59" t="n">
-        <v>0.4259239069249567</v>
+        <v>0.4017743734968386</v>
       </c>
       <c r="D59" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="60">
@@ -1272,13 +1272,13 @@
         <v>290</v>
       </c>
       <c r="B60" t="n">
-        <v>0.09277888576767558</v>
+        <v>0.1153943037206315</v>
       </c>
       <c r="C60" t="n">
-        <v>0.4244592418266188</v>
+        <v>0.3999690296127018</v>
       </c>
       <c r="D60" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="61">
@@ -1286,13 +1286,13 @@
         <v>295</v>
       </c>
       <c r="B61" t="n">
-        <v>0.09325661387629319</v>
+        <v>0.1159634439875716</v>
       </c>
       <c r="C61" t="n">
-        <v>0.4239815137180011</v>
+        <v>0.3993998893457616</v>
       </c>
       <c r="D61" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="62">
@@ -1300,13 +1300,13 @@
         <v>300</v>
       </c>
       <c r="B62" t="n">
-        <v>0.09207016597081193</v>
+        <v>0.1145025011203751</v>
       </c>
       <c r="C62" t="n">
-        <v>0.4251679616234824</v>
+        <v>0.4008608322129582</v>
       </c>
       <c r="D62" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="63">
@@ -1314,13 +1314,13 @@
         <v>305</v>
       </c>
       <c r="B63" t="n">
-        <v>0.09053040085504137</v>
+        <v>0.1126187965768652</v>
       </c>
       <c r="C63" t="n">
-        <v>0.4267077267392529</v>
+        <v>0.4027445367564681</v>
       </c>
       <c r="D63" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="64">
@@ -1328,13 +1328,13 @@
         <v>310</v>
       </c>
       <c r="B64" t="n">
-        <v>0.08870670574677467</v>
+        <v>0.1104016073002693</v>
       </c>
       <c r="C64" t="n">
-        <v>0.4285314218475197</v>
+        <v>0.404961726033064</v>
       </c>
       <c r="D64" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="65">
@@ -1342,13 +1342,13 @@
         <v>315</v>
       </c>
       <c r="B65" t="n">
-        <v>0.08840113265900595</v>
+        <v>0.1100378258078877</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4288369949352884</v>
+        <v>0.4053255075254456</v>
       </c>
       <c r="D65" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="66">
@@ -1356,13 +1356,13 @@
         <v>320</v>
       </c>
       <c r="B66" t="n">
-        <v>0.08534522371081214</v>
+        <v>0.1063158628727837</v>
       </c>
       <c r="C66" t="n">
-        <v>0.4318929038834822</v>
+        <v>0.4090474704605496</v>
       </c>
       <c r="D66" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="67">
@@ -1370,13 +1370,13 @@
         <v>325</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0828062826271006</v>
+        <v>0.103239426347126</v>
       </c>
       <c r="C67" t="n">
-        <v>0.4344318449671937</v>
+        <v>0.4121239069862073</v>
       </c>
       <c r="D67" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="68">
@@ -1384,13 +1384,13 @@
         <v>330</v>
       </c>
       <c r="B68" t="n">
-        <v>0.08046759450012785</v>
+        <v>0.1003834769446643</v>
       </c>
       <c r="C68" t="n">
-        <v>0.4367705330941665</v>
+        <v>0.414979856388669</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="69">
@@ -1398,13 +1398,13 @@
         <v>335</v>
       </c>
       <c r="B69" t="n">
-        <v>0.07950968253770516</v>
+        <v>0.09924421177833848</v>
       </c>
       <c r="C69" t="n">
-        <v>0.4377284450565891</v>
+        <v>0.4161191215549948</v>
       </c>
       <c r="D69" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="70">
@@ -1412,13 +1412,13 @@
         <v>340</v>
       </c>
       <c r="B70" t="n">
-        <v>0.07714956535032495</v>
+        <v>0.09638238249003618</v>
       </c>
       <c r="C70" t="n">
-        <v>0.4400885622439694</v>
+        <v>0.4189809508432971</v>
       </c>
       <c r="D70" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="71">
@@ -1426,13 +1426,13 @@
         <v>345</v>
       </c>
       <c r="B71" t="n">
-        <v>0.07435285572916518</v>
+        <v>0.09292443949702987</v>
       </c>
       <c r="C71" t="n">
-        <v>0.4428852718651292</v>
+        <v>0.4224388938363034</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="72">
@@ -1440,13 +1440,13 @@
         <v>350</v>
       </c>
       <c r="B72" t="n">
-        <v>0.07269587025566816</v>
+        <v>0.09097671954341426</v>
       </c>
       <c r="C72" t="n">
-        <v>0.4445422573386262</v>
+        <v>0.424386613789919</v>
       </c>
       <c r="D72" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="73">
@@ -1454,13 +1454,13 @@
         <v>355</v>
       </c>
       <c r="B73" t="n">
-        <v>0.07197240713364636</v>
+        <v>0.09005430396196797</v>
       </c>
       <c r="C73" t="n">
-        <v>0.4452657204606479</v>
+        <v>0.4253090293713653</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="74">
@@ -1468,3037 +1468,1861 @@
         <v>360</v>
       </c>
       <c r="B74" t="n">
-        <v>0.06904672518569441</v>
+        <v>0.08640561405358929</v>
       </c>
       <c r="C74" t="n">
-        <v>0.4481914024085999</v>
+        <v>0.428957719279744</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B75" t="n">
-        <v>0.06809215020464239</v>
+        <v>0.08186664484504021</v>
       </c>
       <c r="C75" t="n">
-        <v>0.449145977389652</v>
+        <v>0.4334966884882931</v>
       </c>
       <c r="D75" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="B76" t="n">
-        <v>0.06535869181765437</v>
+        <v>0.07677391758383391</v>
       </c>
       <c r="C76" t="n">
-        <v>0.45187943577664</v>
+        <v>0.4385894157494994</v>
       </c>
       <c r="D76" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="B77" t="n">
-        <v>0.06307803852437815</v>
+        <v>0.07429010040710959</v>
       </c>
       <c r="C77" t="n">
-        <v>0.4541600890699162</v>
+        <v>0.4410732329262237</v>
       </c>
       <c r="D77" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0612644416588471</v>
+        <v>0.07110225809613818</v>
       </c>
       <c r="C78" t="n">
-        <v>0.4559736859354472</v>
+        <v>0.4442610752371951</v>
       </c>
       <c r="D78" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>385</v>
+        <v>410</v>
       </c>
       <c r="B79" t="n">
-        <v>0.05825921350235234</v>
+        <v>0.07042542499309372</v>
       </c>
       <c r="C79" t="n">
-        <v>0.458978914091942</v>
+        <v>0.4449379083402396</v>
       </c>
       <c r="D79" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>390</v>
+        <v>420</v>
       </c>
       <c r="B80" t="n">
-        <v>0.05929067611543044</v>
+        <v>0.06731782559416846</v>
       </c>
       <c r="C80" t="n">
-        <v>0.4579474514788639</v>
+        <v>0.4480455077391648</v>
       </c>
       <c r="D80" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>395</v>
+        <v>430</v>
       </c>
       <c r="B81" t="n">
-        <v>0.05893860685399004</v>
+        <v>0.06510627581511522</v>
       </c>
       <c r="C81" t="n">
-        <v>0.4582995207403043</v>
+        <v>0.4502570575182181</v>
       </c>
       <c r="D81" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>400</v>
+        <v>440</v>
       </c>
       <c r="B82" t="n">
-        <v>0.05670919266538976</v>
+        <v>0.06204131594925425</v>
       </c>
       <c r="C82" t="n">
-        <v>0.4605289349289046</v>
+        <v>0.453322017384079</v>
       </c>
       <c r="D82" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>405</v>
+        <v>450</v>
       </c>
       <c r="B83" t="n">
-        <v>0.05697205589760904</v>
+        <v>0.05975812648644877</v>
       </c>
       <c r="C83" t="n">
-        <v>0.4602660716966853</v>
+        <v>0.4556052068468845</v>
       </c>
       <c r="D83" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>410</v>
+        <v>460</v>
       </c>
       <c r="B84" t="n">
-        <v>0.05614191420643433</v>
+        <v>0.05814704952813776</v>
       </c>
       <c r="C84" t="n">
-        <v>0.46109621338786</v>
+        <v>0.4572162838051955</v>
       </c>
       <c r="D84" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>415</v>
+        <v>470</v>
       </c>
       <c r="B85" t="n">
-        <v>0.05349352232353648</v>
+        <v>0.05584306193899476</v>
       </c>
       <c r="C85" t="n">
-        <v>0.4637446052707578</v>
+        <v>0.4595202713943385</v>
       </c>
       <c r="D85" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>420</v>
+        <v>480</v>
       </c>
       <c r="B86" t="n">
-        <v>0.05364577693132419</v>
+        <v>0.05460259601930655</v>
       </c>
       <c r="C86" t="n">
-        <v>0.4635923506629701</v>
+        <v>0.4607607373140267</v>
       </c>
       <c r="D86" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>425</v>
+        <v>490</v>
       </c>
       <c r="B87" t="n">
-        <v>0.05261032339407166</v>
+        <v>0.05237073579206617</v>
       </c>
       <c r="C87" t="n">
-        <v>0.4646278042002226</v>
+        <v>0.4629925975412671</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>430</v>
+        <v>500</v>
       </c>
       <c r="B88" t="n">
-        <v>0.05188964897419562</v>
+        <v>0.05225315910831347</v>
       </c>
       <c r="C88" t="n">
-        <v>0.4653484786200987</v>
+        <v>0.4631101742250198</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>435</v>
+        <v>510</v>
       </c>
       <c r="B89" t="n">
-        <v>0.04965420768326074</v>
+        <v>0.05144347049305583</v>
       </c>
       <c r="C89" t="n">
-        <v>0.4675839199110336</v>
+        <v>0.4639198628402775</v>
       </c>
       <c r="D89" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>440</v>
+        <v>520</v>
       </c>
       <c r="B90" t="n">
-        <v>0.0494121912645389</v>
+        <v>0.04996492186633172</v>
       </c>
       <c r="C90" t="n">
-        <v>0.4678259363297554</v>
+        <v>0.4653984114670016</v>
       </c>
       <c r="D90" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>445</v>
+        <v>530</v>
       </c>
       <c r="B91" t="n">
-        <v>0.04854564407293265</v>
+        <v>0.04823669888420021</v>
       </c>
       <c r="C91" t="n">
-        <v>0.4686924835213617</v>
+        <v>0.467126634449133</v>
       </c>
       <c r="D91" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>450</v>
+        <v>540</v>
       </c>
       <c r="B92" t="n">
-        <v>0.04761058814290031</v>
+        <v>0.04514689803647191</v>
       </c>
       <c r="C92" t="n">
-        <v>0.469627539451394</v>
+        <v>0.4702164352968614</v>
       </c>
       <c r="D92" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>455</v>
+        <v>550</v>
       </c>
       <c r="B93" t="n">
-        <v>0.04741282358526211</v>
+        <v>0.04147875798366313</v>
       </c>
       <c r="C93" t="n">
-        <v>0.4698253040090322</v>
+        <v>0.4738845753496702</v>
       </c>
       <c r="D93" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>460</v>
+        <v>560</v>
       </c>
       <c r="B94" t="n">
-        <v>0.04631193480126454</v>
+        <v>0.03846241657465899</v>
       </c>
       <c r="C94" t="n">
-        <v>0.4709261927930298</v>
+        <v>0.4769009167586743</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>465</v>
+        <v>570</v>
       </c>
       <c r="B95" t="n">
-        <v>0.04557521199373989</v>
+        <v>0.03900862780068563</v>
       </c>
       <c r="C95" t="n">
-        <v>0.4716629156005545</v>
+        <v>0.4763547055326476</v>
       </c>
       <c r="D95" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>470</v>
+        <v>580</v>
       </c>
       <c r="B96" t="n">
-        <v>0.04445183740571355</v>
+        <v>0.03919995566288261</v>
       </c>
       <c r="C96" t="n">
-        <v>0.4727862901885808</v>
+        <v>0.4761633776704507</v>
       </c>
       <c r="D96" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>475</v>
+        <v>590</v>
       </c>
       <c r="B97" t="n">
-        <v>0.04446479072263266</v>
+        <v>0.03738707570811919</v>
       </c>
       <c r="C97" t="n">
-        <v>0.4727733368716617</v>
+        <v>0.4779762576252141</v>
       </c>
       <c r="D97" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="B98" t="n">
-        <v>0.04345609176827094</v>
+        <v>0.03623271647231331</v>
       </c>
       <c r="C98" t="n">
-        <v>0.4737820358260234</v>
+        <v>0.47913061686102</v>
       </c>
       <c r="D98" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>485</v>
+        <v>610</v>
       </c>
       <c r="B99" t="n">
-        <v>0.04351415178048695</v>
+        <v>0.03389087804897215</v>
       </c>
       <c r="C99" t="n">
-        <v>0.4737239758138074</v>
+        <v>0.4814724552843611</v>
       </c>
       <c r="D99" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>490</v>
+        <v>620</v>
       </c>
       <c r="B100" t="n">
-        <v>0.04169649334277276</v>
+        <v>0.03229591800081596</v>
       </c>
       <c r="C100" t="n">
-        <v>0.4755416342515216</v>
+        <v>0.4830674153325173</v>
       </c>
       <c r="D100" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>495</v>
+        <v>630</v>
       </c>
       <c r="B101" t="n">
-        <v>0.04152111774817004</v>
+        <v>0.03080478002109239</v>
       </c>
       <c r="C101" t="n">
-        <v>0.4757170098461243</v>
+        <v>0.4845585533122409</v>
       </c>
       <c r="D101" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>500</v>
+        <v>640</v>
       </c>
       <c r="B102" t="n">
-        <v>0.04160733490493601</v>
+        <v>0.02755390921223462</v>
       </c>
       <c r="C102" t="n">
-        <v>0.4756307926893583</v>
+        <v>0.4878094241210987</v>
       </c>
       <c r="D102" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>505</v>
+        <v>650</v>
       </c>
       <c r="B103" t="n">
-        <v>0.04148306685099049</v>
+        <v>0.02629405561471225</v>
       </c>
       <c r="C103" t="n">
-        <v>0.4757550607433039</v>
+        <v>0.489069277718621</v>
       </c>
       <c r="D103" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>510</v>
+        <v>660</v>
       </c>
       <c r="B104" t="n">
-        <v>0.0409596369100843</v>
+        <v>0.02558003730165804</v>
       </c>
       <c r="C104" t="n">
-        <v>0.47627849068421</v>
+        <v>0.4897832960316753</v>
       </c>
       <c r="D104" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>515</v>
+        <v>670</v>
       </c>
       <c r="B105" t="n">
-        <v>0.04033199014486484</v>
+        <v>0.02450459913056754</v>
       </c>
       <c r="C105" t="n">
-        <v>0.4769061374494295</v>
+        <v>0.4908587342027658</v>
       </c>
       <c r="D105" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>520</v>
+        <v>680</v>
       </c>
       <c r="B106" t="n">
-        <v>0.03975982489602103</v>
+        <v>0.02398085768956935</v>
       </c>
       <c r="C106" t="n">
-        <v>0.4774783026982733</v>
+        <v>0.4913824756437639</v>
       </c>
       <c r="D106" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>525</v>
+        <v>690</v>
       </c>
       <c r="B107" t="n">
-        <v>0.03965305749284414</v>
+        <v>0.02286802765199221</v>
       </c>
       <c r="C107" t="n">
-        <v>0.4775850701014502</v>
+        <v>0.4924953056813411</v>
       </c>
       <c r="D107" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>530</v>
+        <v>700</v>
       </c>
       <c r="B108" t="n">
-        <v>0.0383801038855771</v>
+        <v>0.02185518230578065</v>
       </c>
       <c r="C108" t="n">
-        <v>0.4788580237087172</v>
+        <v>0.4935081510275526</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>535</v>
+        <v>710</v>
       </c>
       <c r="B109" t="n">
-        <v>0.03814622116691229</v>
+        <v>0.02103353500400883</v>
       </c>
       <c r="C109" t="n">
-        <v>0.479091906427382</v>
+        <v>0.4943297983293244</v>
       </c>
       <c r="D109" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>540</v>
+        <v>720</v>
       </c>
       <c r="B110" t="n">
-        <v>0.03583175311509197</v>
+        <v>0.02072648604379955</v>
       </c>
       <c r="C110" t="n">
-        <v>0.4814063744792024</v>
+        <v>0.4946368472895337</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>545</v>
+        <v>730</v>
       </c>
       <c r="B111" t="n">
-        <v>0.0351158577028878</v>
+        <v>0.02074700932210514</v>
       </c>
       <c r="C111" t="n">
-        <v>0.4821222698914066</v>
+        <v>0.4946163240112281</v>
       </c>
       <c r="D111" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>550</v>
+        <v>740</v>
       </c>
       <c r="B112" t="n">
-        <v>0.03292813241895458</v>
+        <v>0.01986536991859419</v>
       </c>
       <c r="C112" t="n">
-        <v>0.4843099951753397</v>
+        <v>0.4954979634147391</v>
       </c>
       <c r="D112" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>555</v>
+        <v>750</v>
       </c>
       <c r="B113" t="n">
-        <v>0.03026197351274683</v>
+        <v>0.01918533961795687</v>
       </c>
       <c r="C113" t="n">
-        <v>0.4869761540815475</v>
+        <v>0.4961779937153764</v>
       </c>
       <c r="D113" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>560</v>
+        <v>760</v>
       </c>
       <c r="B114" t="n">
-        <v>0.03049336730680929</v>
+        <v>0.01859924959622642</v>
       </c>
       <c r="C114" t="n">
-        <v>0.486744760287485</v>
+        <v>0.4967640837371068</v>
       </c>
       <c r="D114" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>565</v>
+        <v>770</v>
       </c>
       <c r="B115" t="n">
-        <v>0.03123201384289925</v>
+        <v>0.01578346008900833</v>
       </c>
       <c r="C115" t="n">
-        <v>0.4860061137513951</v>
+        <v>0.499579873244325</v>
       </c>
       <c r="D115" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>570</v>
+        <v>780</v>
       </c>
       <c r="B116" t="n">
-        <v>0.03093946653124831</v>
+        <v>0.01530452119793228</v>
       </c>
       <c r="C116" t="n">
-        <v>0.486298661063046</v>
+        <v>0.500058812135401</v>
       </c>
       <c r="D116" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>575</v>
+        <v>790</v>
       </c>
       <c r="B117" t="n">
-        <v>0.03123490714833049</v>
+        <v>0.0150563390097622</v>
       </c>
       <c r="C117" t="n">
-        <v>0.4860032204459638</v>
+        <v>0.5003069943235711</v>
       </c>
       <c r="D117" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>580</v>
+        <v>800</v>
       </c>
       <c r="B118" t="n">
-        <v>0.03108146945400639</v>
+        <v>0.01440699078072755</v>
       </c>
       <c r="C118" t="n">
-        <v>0.4861566581402879</v>
+        <v>0.5009563425526057</v>
       </c>
       <c r="D118" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>585</v>
+        <v>810</v>
       </c>
       <c r="B119" t="n">
-        <v>0.03074776734307665</v>
+        <v>0.01412016414660462</v>
       </c>
       <c r="C119" t="n">
-        <v>0.4864903602512177</v>
+        <v>0.5012431691867286</v>
       </c>
       <c r="D119" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>590</v>
+        <v>820</v>
       </c>
       <c r="B120" t="n">
-        <v>0.02963355332921335</v>
+        <v>0.01409968279079973</v>
       </c>
       <c r="C120" t="n">
-        <v>0.487604574265081</v>
+        <v>0.5012636505425335</v>
       </c>
       <c r="D120" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>595</v>
+        <v>830</v>
       </c>
       <c r="B121" t="n">
-        <v>0.02916034967234275</v>
+        <v>0.01308569890356427</v>
       </c>
       <c r="C121" t="n">
-        <v>0.4880777779219516</v>
+        <v>0.502277634429769</v>
       </c>
       <c r="D121" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>600</v>
+        <v>840</v>
       </c>
       <c r="B122" t="n">
-        <v>0.02873745391303436</v>
+        <v>0.01300139497003213</v>
       </c>
       <c r="C122" t="n">
-        <v>0.48850067368126</v>
+        <v>0.5023619383633011</v>
       </c>
       <c r="D122" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>605</v>
+        <v>850</v>
       </c>
       <c r="B123" t="n">
-        <v>0.02797901696408638</v>
+        <v>0.01243656360356796</v>
       </c>
       <c r="C123" t="n">
-        <v>0.4892591106302079</v>
+        <v>0.5029267697297654</v>
       </c>
       <c r="D123" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>610</v>
+        <v>860</v>
       </c>
       <c r="B124" t="n">
-        <v>0.02691307100124143</v>
+        <v>0.01170232056233504</v>
       </c>
       <c r="C124" t="n">
-        <v>0.4903250565930529</v>
+        <v>0.5036610127709983</v>
       </c>
       <c r="D124" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>615</v>
+        <v>870</v>
       </c>
       <c r="B125" t="n">
-        <v>0.02685021983144822</v>
+        <v>0.01131269823515108</v>
       </c>
       <c r="C125" t="n">
-        <v>0.4903879077628461</v>
+        <v>0.5040506350981822</v>
       </c>
       <c r="D125" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>620</v>
+        <v>880</v>
       </c>
       <c r="B126" t="n">
-        <v>0.02564724725533918</v>
+        <v>0.01207604050481748</v>
       </c>
       <c r="C126" t="n">
-        <v>0.4915908803389551</v>
+        <v>0.5032872928285158</v>
       </c>
       <c r="D126" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>625</v>
+        <v>890</v>
       </c>
       <c r="B127" t="n">
-        <v>0.0254629117081412</v>
+        <v>0.01166843582544226</v>
       </c>
       <c r="C127" t="n">
-        <v>0.4917752158861531</v>
+        <v>0.503694897507891</v>
       </c>
       <c r="D127" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>630</v>
+        <v>900</v>
       </c>
       <c r="B128" t="n">
-        <v>0.02449600280037568</v>
+        <v>0.01124902979809336</v>
       </c>
       <c r="C128" t="n">
-        <v>0.4927421247939187</v>
+        <v>0.5041143035352399</v>
       </c>
       <c r="D128" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>635</v>
+        <v>910</v>
       </c>
       <c r="B129" t="n">
-        <v>0.02189813944178791</v>
+        <v>0.01229163582180081</v>
       </c>
       <c r="C129" t="n">
-        <v>0.4953399881525064</v>
+        <v>0.5030716975115325</v>
       </c>
       <c r="D129" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>640</v>
+        <v>920</v>
       </c>
       <c r="B130" t="n">
-        <v>0.02190681571722606</v>
+        <v>0.01182249269947247</v>
       </c>
       <c r="C130" t="n">
-        <v>0.4953313118770682</v>
+        <v>0.5035408406338608</v>
       </c>
       <c r="D130" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>645</v>
+        <v>930</v>
       </c>
       <c r="B131" t="n">
-        <v>0.02149821382929612</v>
+        <v>0.01181493030958819</v>
       </c>
       <c r="C131" t="n">
-        <v>0.4957399137649982</v>
+        <v>0.503548403023745</v>
       </c>
       <c r="D131" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>650</v>
+        <v>940</v>
       </c>
       <c r="B132" t="n">
-        <v>0.0208807402100992</v>
+        <v>0.0107348710537367</v>
       </c>
       <c r="C132" t="n">
-        <v>0.4963573873841951</v>
+        <v>0.5046284622795966</v>
       </c>
       <c r="D132" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>655</v>
+        <v>950</v>
       </c>
       <c r="B133" t="n">
-        <v>0.02046543676981875</v>
+        <v>0.01031667857251948</v>
       </c>
       <c r="C133" t="n">
-        <v>0.4967726908244756</v>
+        <v>0.5050466547608138</v>
       </c>
       <c r="D133" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>660</v>
+        <v>960</v>
       </c>
       <c r="B134" t="n">
-        <v>0.02030293929794115</v>
+        <v>0.01004326660829759</v>
       </c>
       <c r="C134" t="n">
-        <v>0.4969351882963532</v>
+        <v>0.5053200667250357</v>
       </c>
       <c r="D134" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>665</v>
+        <v>970</v>
       </c>
       <c r="B135" t="n">
-        <v>0.0201758459397972</v>
+        <v>0.008080158448111526</v>
       </c>
       <c r="C135" t="n">
-        <v>0.4970622816544971</v>
+        <v>0.5072831748852218</v>
       </c>
       <c r="D135" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>670</v>
+        <v>980</v>
       </c>
       <c r="B136" t="n">
-        <v>0.0194486038633688</v>
+        <v>0.007106381645886</v>
       </c>
       <c r="C136" t="n">
-        <v>0.4977895237309256</v>
+        <v>0.5082569516874473</v>
       </c>
       <c r="D136" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>675</v>
+        <v>990</v>
       </c>
       <c r="B137" t="n">
-        <v>0.01907726424189165</v>
+        <v>0.005659196580002844</v>
       </c>
       <c r="C137" t="n">
-        <v>0.4981608633524027</v>
+        <v>0.5097041367533305</v>
       </c>
       <c r="D137" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>680</v>
+        <v>1000</v>
       </c>
       <c r="B138" t="n">
-        <v>0.01903647890506558</v>
+        <v>0.005450771355050327</v>
       </c>
       <c r="C138" t="n">
-        <v>0.4982016486892287</v>
+        <v>0.5099125619782829</v>
       </c>
       <c r="D138" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>685</v>
+        <v>1010</v>
       </c>
       <c r="B139" t="n">
-        <v>0.01856210652236734</v>
+        <v>0.005301152112409586</v>
       </c>
       <c r="C139" t="n">
-        <v>0.498676021071927</v>
+        <v>0.5100621812209237</v>
       </c>
       <c r="D139" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>690</v>
+        <v>1020</v>
       </c>
       <c r="B140" t="n">
-        <v>0.01815986755427028</v>
+        <v>0.005066808523795245</v>
       </c>
       <c r="C140" t="n">
-        <v>0.499078260040024</v>
+        <v>0.510296524809538</v>
       </c>
       <c r="D140" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>695</v>
+        <v>1030</v>
       </c>
       <c r="B141" t="n">
-        <v>0.01746815300398813</v>
+        <v>0.005222261549429203</v>
       </c>
       <c r="C141" t="n">
-        <v>0.4997699745903062</v>
+        <v>0.5101410717839041</v>
       </c>
       <c r="D141" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>700</v>
+        <v>1040</v>
       </c>
       <c r="B142" t="n">
-        <v>0.01734941624589357</v>
+        <v>0.00499076029375033</v>
       </c>
       <c r="C142" t="n">
-        <v>0.4998887113484007</v>
+        <v>0.5103725730395829</v>
       </c>
       <c r="D142" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>705</v>
+        <v>1050</v>
       </c>
       <c r="B143" t="n">
-        <v>0.01705965386869107</v>
+        <v>0.005055652398685087</v>
       </c>
       <c r="C143" t="n">
-        <v>0.5001784737256032</v>
+        <v>0.5103076809346482</v>
       </c>
       <c r="D143" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>710</v>
+        <v>1060</v>
       </c>
       <c r="B144" t="n">
-        <v>0.01669223225660003</v>
+        <v>0.004896895594736743</v>
       </c>
       <c r="C144" t="n">
-        <v>0.5005458953376943</v>
+        <v>0.5104664377385966</v>
       </c>
       <c r="D144" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>715</v>
+        <v>1070</v>
       </c>
       <c r="B145" t="n">
-        <v>0.01663730724687532</v>
+        <v>0.005138239658177334</v>
       </c>
       <c r="C145" t="n">
-        <v>0.500600820347419</v>
+        <v>0.510225093675156</v>
       </c>
       <c r="D145" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="B146" t="n">
-        <v>0.01644871816812546</v>
+        <v>0.005257094769990193</v>
       </c>
       <c r="C146" t="n">
-        <v>0.5007894094261689</v>
+        <v>0.5101062385633431</v>
       </c>
       <c r="D146" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>725</v>
+        <v>1090</v>
       </c>
       <c r="B147" t="n">
-        <v>0.01659409118021324</v>
+        <v>0.005162875112013281</v>
       </c>
       <c r="C147" t="n">
-        <v>0.5006440364140811</v>
+        <v>0.51020045822132</v>
       </c>
       <c r="D147" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>730</v>
+        <v>1100</v>
       </c>
       <c r="B148" t="n">
-        <v>0.01645884275449066</v>
+        <v>0.005524752238268719</v>
       </c>
       <c r="C148" t="n">
-        <v>0.5007792848398037</v>
+        <v>0.5098385810950645</v>
       </c>
       <c r="D148" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>735</v>
+        <v>1110</v>
       </c>
       <c r="B149" t="n">
-        <v>0.01625136677576831</v>
+        <v>0.005448793571852992</v>
       </c>
       <c r="C149" t="n">
-        <v>0.500986760818526</v>
+        <v>0.5099145397614803</v>
       </c>
       <c r="D149" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>740</v>
+        <v>1120</v>
       </c>
       <c r="B150" t="n">
-        <v>0.01575058140834213</v>
+        <v>0.005636409519954828</v>
       </c>
       <c r="C150" t="n">
-        <v>0.5014875461859521</v>
+        <v>0.5097269238133785</v>
       </c>
       <c r="D150" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>745</v>
+        <v>1130</v>
       </c>
       <c r="B151" t="n">
-        <v>0.01560045941960845</v>
+        <v>0.00537115323953287</v>
       </c>
       <c r="C151" t="n">
-        <v>0.5016376681746859</v>
+        <v>0.5099921800938004</v>
       </c>
       <c r="D151" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>750</v>
+        <v>1140</v>
       </c>
       <c r="B152" t="n">
-        <v>0.01520872733551301</v>
+        <v>0.005178630684522441</v>
       </c>
       <c r="C152" t="n">
-        <v>0.5020294002587813</v>
+        <v>0.5101847026488109</v>
       </c>
       <c r="D152" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>755</v>
+        <v>1150</v>
       </c>
       <c r="B153" t="n">
-        <v>0.01489965676307436</v>
+        <v>0.005120802215316471</v>
       </c>
       <c r="C153" t="n">
-        <v>0.50233847083122</v>
+        <v>0.5102425311180168</v>
       </c>
       <c r="D153" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>760</v>
+        <v>1160</v>
       </c>
       <c r="B154" t="n">
-        <v>0.0147358683627395</v>
+        <v>0.00519414474471646</v>
       </c>
       <c r="C154" t="n">
-        <v>0.5025022592315548</v>
+        <v>0.5101691885886168</v>
       </c>
       <c r="D154" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>765</v>
+        <v>1170</v>
       </c>
       <c r="B155" t="n">
-        <v>0.01453428902891305</v>
+        <v>0.004978228613015481</v>
       </c>
       <c r="C155" t="n">
-        <v>0.5027038385653813</v>
+        <v>0.5103851047203178</v>
       </c>
       <c r="D155" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>770</v>
+        <v>1180</v>
       </c>
       <c r="B156" t="n">
-        <v>0.01243860607584214</v>
+        <v>0.004550394240590331</v>
       </c>
       <c r="C156" t="n">
-        <v>0.5047995215184522</v>
+        <v>0.5108129390927429</v>
       </c>
       <c r="D156" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>775</v>
+        <v>1190</v>
       </c>
       <c r="B157" t="n">
-        <v>0.01242844101214062</v>
+        <v>0.004453137618437959</v>
       </c>
       <c r="C157" t="n">
-        <v>0.5048096865821537</v>
+        <v>0.5109101957148954</v>
       </c>
       <c r="D157" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>780</v>
+        <v>1200</v>
       </c>
       <c r="B158" t="n">
-        <v>0.01205928074132718</v>
+        <v>0.004362454846293924</v>
       </c>
       <c r="C158" t="n">
-        <v>0.5051788468529671</v>
+        <v>0.5110008784870393</v>
       </c>
       <c r="D158" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>785</v>
+        <v>1210</v>
       </c>
       <c r="B159" t="n">
-        <v>0.01188905290300663</v>
+        <v>0.004644448841453261</v>
       </c>
       <c r="C159" t="n">
-        <v>0.5053490746912876</v>
+        <v>0.5107188844918801</v>
       </c>
       <c r="D159" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>790</v>
+        <v>1220</v>
       </c>
       <c r="B160" t="n">
-        <v>0.01185942691832404</v>
+        <v>0.004321208207765203</v>
       </c>
       <c r="C160" t="n">
-        <v>0.5053787006759702</v>
+        <v>0.5110421251255681</v>
       </c>
       <c r="D160" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>795</v>
+        <v>1230</v>
       </c>
       <c r="B161" t="n">
-        <v>0.0115726526183652</v>
+        <v>0.004147657479759407</v>
       </c>
       <c r="C161" t="n">
-        <v>0.5056654749759292</v>
+        <v>0.5112156758535739</v>
       </c>
       <c r="D161" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>800</v>
+        <v>1240</v>
       </c>
       <c r="B162" t="n">
-        <v>0.01134236703100423</v>
+        <v>0.004096383408035648</v>
       </c>
       <c r="C162" t="n">
-        <v>0.5058957605632901</v>
+        <v>0.5112669499252976</v>
       </c>
       <c r="D162" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>805</v>
+        <v>1250</v>
       </c>
       <c r="B163" t="n">
-        <v>0.01119281177219333</v>
+        <v>0.003842821627708453</v>
       </c>
       <c r="C163" t="n">
-        <v>0.506045315822101</v>
+        <v>0.5115205117056248</v>
       </c>
       <c r="D163" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>810</v>
+        <v>1260</v>
       </c>
       <c r="B164" t="n">
-        <v>0.01110968654328464</v>
+        <v>0.003986220161279353</v>
       </c>
       <c r="C164" t="n">
-        <v>0.5061284410510097</v>
+        <v>0.5113771131720539</v>
       </c>
       <c r="D164" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>815</v>
+        <v>1270</v>
       </c>
       <c r="B165" t="n">
-        <v>0.0110625715288515</v>
+        <v>0.003847586395017633</v>
       </c>
       <c r="C165" t="n">
-        <v>0.5061755560654428</v>
+        <v>0.5115157469383157</v>
       </c>
       <c r="D165" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>820</v>
+        <v>1280</v>
       </c>
       <c r="B166" t="n">
-        <v>0.01109410534326588</v>
+        <v>0.00380628985017411</v>
       </c>
       <c r="C166" t="n">
-        <v>0.5061440222510285</v>
+        <v>0.5115570434831592</v>
       </c>
       <c r="D166" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>825</v>
+        <v>1290</v>
       </c>
       <c r="B167" t="n">
-        <v>0.01089665424377843</v>
+        <v>0.00383565609105755</v>
       </c>
       <c r="C167" t="n">
-        <v>0.5063414733505159</v>
+        <v>0.5115276772422758</v>
       </c>
       <c r="D167" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>830</v>
+        <v>1300</v>
       </c>
       <c r="B168" t="n">
-        <v>0.01029389163682945</v>
+        <v>0.003840293121675145</v>
       </c>
       <c r="C168" t="n">
-        <v>0.5069442359574649</v>
+        <v>0.5115230402116582</v>
       </c>
       <c r="D168" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>835</v>
+        <v>1310</v>
       </c>
       <c r="B169" t="n">
-        <v>0.01035438158732253</v>
+        <v>0.003829041400799446</v>
       </c>
       <c r="C169" t="n">
-        <v>0.5068837460069718</v>
+        <v>0.5115342919325339</v>
       </c>
       <c r="D169" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>840</v>
+        <v>1320</v>
       </c>
       <c r="B170" t="n">
-        <v>0.01022051041392779</v>
+        <v>0.00385792015474899</v>
       </c>
       <c r="C170" t="n">
-        <v>0.5070176171803665</v>
+        <v>0.5115054131785843</v>
       </c>
       <c r="D170" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>845</v>
+        <v>1330</v>
       </c>
       <c r="B171" t="n">
-        <v>0.01000188846348392</v>
+        <v>0.003871251880444085</v>
       </c>
       <c r="C171" t="n">
-        <v>0.5072362391308104</v>
+        <v>0.5114920814528892</v>
       </c>
       <c r="D171" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>850</v>
+        <v>1340</v>
       </c>
       <c r="B172" t="n">
-        <v>0.009762844667666247</v>
+        <v>0.003824984879972825</v>
       </c>
       <c r="C172" t="n">
-        <v>0.5074752829266281</v>
+        <v>0.5115383484533604</v>
       </c>
       <c r="D172" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>855</v>
+        <v>1350</v>
       </c>
       <c r="B173" t="n">
-        <v>0.009599173756760292</v>
+        <v>0.00386388432586906</v>
       </c>
       <c r="C173" t="n">
-        <v>0.507638953837534</v>
+        <v>0.5114994490074642</v>
       </c>
       <c r="D173" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>860</v>
+        <v>1360</v>
       </c>
       <c r="B174" t="n">
-        <v>0.009178982501795337</v>
+        <v>0.004083744461197319</v>
       </c>
       <c r="C174" t="n">
-        <v>0.5080591450924989</v>
+        <v>0.511279588872136</v>
       </c>
       <c r="D174" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>865</v>
+        <v>1370</v>
       </c>
       <c r="B175" t="n">
-        <v>0.009280855363314846</v>
+        <v>0.003884691220348778</v>
       </c>
       <c r="C175" t="n">
-        <v>0.5079572722309795</v>
+        <v>0.5114786421129845</v>
       </c>
       <c r="D175" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>870</v>
+        <v>1380</v>
       </c>
       <c r="B176" t="n">
-        <v>0.008859430288549505</v>
+        <v>0.003924505234605824</v>
       </c>
       <c r="C176" t="n">
-        <v>0.5083786973057448</v>
+        <v>0.5114388280987274</v>
       </c>
       <c r="D176" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>875</v>
+        <v>1390</v>
       </c>
       <c r="B177" t="n">
-        <v>0.009038649436687583</v>
+        <v>0.003843850647032152</v>
       </c>
       <c r="C177" t="n">
-        <v>0.5081994781576068</v>
+        <v>0.5115194826863011</v>
       </c>
       <c r="D177" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>880</v>
+        <v>1400</v>
       </c>
       <c r="B178" t="n">
-        <v>0.009481754959824461</v>
+        <v>0.003844226254063731</v>
       </c>
       <c r="C178" t="n">
-        <v>0.5077563726344698</v>
+        <v>0.5115191070792695</v>
       </c>
       <c r="D178" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>885</v>
+        <v>1410</v>
       </c>
       <c r="B179" t="n">
-        <v>0.009474325193605483</v>
+        <v>0.003837509932621888</v>
       </c>
       <c r="C179" t="n">
-        <v>0.5077638024006889</v>
+        <v>0.5115258234007114</v>
       </c>
       <c r="D179" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>890</v>
+        <v>1420</v>
       </c>
       <c r="B180" t="n">
-        <v>0.009155263765400701</v>
+        <v>0.003729036292383767</v>
       </c>
       <c r="C180" t="n">
-        <v>0.5080828638288937</v>
+        <v>0.5116342970409495</v>
       </c>
       <c r="D180" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>895</v>
+        <v>1430</v>
       </c>
       <c r="B181" t="n">
-        <v>0.00916282595887744</v>
+        <v>0.003691228633740765</v>
       </c>
       <c r="C181" t="n">
-        <v>0.5080753016354169</v>
+        <v>0.5116721046995926</v>
       </c>
       <c r="D181" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>900</v>
+        <v>1440</v>
       </c>
       <c r="B182" t="n">
-        <v>0.008812417969033114</v>
+        <v>0.003019795958449613</v>
       </c>
       <c r="C182" t="n">
-        <v>0.5084257096252612</v>
+        <v>0.5123435373748837</v>
       </c>
       <c r="D182" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>905</v>
+        <v>1500</v>
       </c>
       <c r="B183" t="n">
-        <v>0.008696824346804414</v>
+        <v>0.003047134517394411</v>
       </c>
       <c r="C183" t="n">
-        <v>0.5085413032474899</v>
+        <v>0.5123161988159389</v>
       </c>
       <c r="D183" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>910</v>
+        <v>1560</v>
       </c>
       <c r="B184" t="n">
-        <v>0.009648070067589427</v>
+        <v>0.003414599993797531</v>
       </c>
       <c r="C184" t="n">
-        <v>0.5075900575267049</v>
+        <v>0.5119487333395357</v>
       </c>
       <c r="D184" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>915</v>
+        <v>1620</v>
       </c>
       <c r="B185" t="n">
-        <v>0.009446601703620092</v>
+        <v>0.003407681197890447</v>
       </c>
       <c r="C185" t="n">
-        <v>0.5077915258906742</v>
+        <v>0.5119556521354428</v>
       </c>
       <c r="D185" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>920</v>
+        <v>1680</v>
       </c>
       <c r="B186" t="n">
-        <v>0.009256834160721381</v>
+        <v>0.003341760398368455</v>
       </c>
       <c r="C186" t="n">
-        <v>0.5079812934335729</v>
+        <v>0.5120215729349649</v>
       </c>
       <c r="D186" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>925</v>
+        <v>1740</v>
       </c>
       <c r="B187" t="n">
-        <v>0.009171715013577206</v>
+        <v>0.003242380567010089</v>
       </c>
       <c r="C187" t="n">
-        <v>0.5080664125807172</v>
+        <v>0.5121209527663232</v>
       </c>
       <c r="D187" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>930</v>
+        <v>1800</v>
       </c>
       <c r="B188" t="n">
-        <v>0.009246366679869457</v>
+        <v>0.003175866929599245</v>
       </c>
       <c r="C188" t="n">
-        <v>0.5079917609144249</v>
+        <v>0.512187466403734</v>
       </c>
       <c r="D188" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>935</v>
+        <v>1860</v>
       </c>
       <c r="B189" t="n">
-        <v>0.008541775580346448</v>
+        <v>0.003245012443459706</v>
       </c>
       <c r="C189" t="n">
-        <v>0.5086963520139479</v>
+        <v>0.5121183208898735</v>
       </c>
       <c r="D189" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>940</v>
+        <v>1920</v>
       </c>
       <c r="B190" t="n">
-        <v>0.008394788022710958</v>
+        <v>0.003168918450861292</v>
       </c>
       <c r="C190" t="n">
-        <v>0.5088433395715833</v>
+        <v>0.512194414882472</v>
       </c>
       <c r="D190" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>945</v>
+        <v>1980</v>
       </c>
       <c r="B191" t="n">
-        <v>0.007969724293270369</v>
+        <v>0.003174188690346376</v>
       </c>
       <c r="C191" t="n">
-        <v>0.509268403301024</v>
+        <v>0.5121891446429869</v>
       </c>
       <c r="D191" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>950</v>
+        <v>2040</v>
       </c>
       <c r="B192" t="n">
-        <v>0.008046507782918917</v>
+        <v>0.003174222892435094</v>
       </c>
       <c r="C192" t="n">
-        <v>0.5091916198113754</v>
+        <v>0.5121891104408982</v>
       </c>
       <c r="D192" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>955</v>
+        <v>2100</v>
       </c>
       <c r="B193" t="n">
-        <v>0.008078177545910229</v>
+        <v>0.00323303609331097</v>
       </c>
       <c r="C193" t="n">
-        <v>0.5091599500483841</v>
+        <v>0.5121302972400223</v>
       </c>
       <c r="D193" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>960</v>
+        <v>2160</v>
       </c>
       <c r="B194" t="n">
-        <v>0.007829062990822653</v>
+        <v>0.003163715625433079</v>
       </c>
       <c r="C194" t="n">
-        <v>0.5094090646034717</v>
+        <v>0.5121996177079002</v>
       </c>
       <c r="D194" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>965</v>
+        <v>2220</v>
       </c>
       <c r="B195" t="n">
-        <v>0.007408536532360259</v>
+        <v>0.003154529102586449</v>
       </c>
       <c r="C195" t="n">
-        <v>0.509829591061934</v>
+        <v>0.5122088042307469</v>
       </c>
       <c r="D195" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>970</v>
+        <v>2280</v>
       </c>
       <c r="B196" t="n">
-        <v>0.006235098291217072</v>
+        <v>0.003059366747621569</v>
       </c>
       <c r="C196" t="n">
-        <v>0.5110030293030773</v>
+        <v>0.5123039665857118</v>
       </c>
       <c r="D196" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>975</v>
+        <v>2340</v>
       </c>
       <c r="B197" t="n">
-        <v>0.005663533069819507</v>
+        <v>0.003048495098253766</v>
       </c>
       <c r="C197" t="n">
-        <v>0.5115745945244748</v>
+        <v>0.5123148382350795</v>
       </c>
       <c r="D197" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>980</v>
+        <v>2400</v>
       </c>
       <c r="B198" t="n">
-        <v>0.005486934991314859</v>
+        <v>0.003106135056899931</v>
       </c>
       <c r="C198" t="n">
-        <v>0.5117511926029795</v>
+        <v>0.5122571982764333</v>
       </c>
       <c r="D198" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>985</v>
+        <v>2460</v>
       </c>
       <c r="B199" t="n">
-        <v>0.004582711261842723</v>
+        <v>0.003042803727651008</v>
       </c>
       <c r="C199" t="n">
-        <v>0.5126554163324516</v>
+        <v>0.5123205296056823</v>
       </c>
       <c r="D199" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>990</v>
+        <v>2520</v>
       </c>
       <c r="B200" t="n">
-        <v>0.004340555281585</v>
+        <v>0.00310089400457784</v>
       </c>
       <c r="C200" t="n">
-        <v>0.5128975723127094</v>
+        <v>0.5122624393287555</v>
       </c>
       <c r="D200" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>995</v>
+        <v>2580</v>
       </c>
       <c r="B201" t="n">
-        <v>0.004152838768085351</v>
+        <v>0.003074486433065403</v>
       </c>
       <c r="C201" t="n">
-        <v>0.513085288826209</v>
+        <v>0.5122888469002679</v>
       </c>
       <c r="D201" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>1000</v>
+        <v>2640</v>
       </c>
       <c r="B202" t="n">
-        <v>0.004174465268844877</v>
+        <v>0.00305637074141317</v>
       </c>
       <c r="C202" t="n">
-        <v>0.5130636623254494</v>
+        <v>0.5123069625919201</v>
       </c>
       <c r="D202" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>1005</v>
+        <v>2700</v>
       </c>
       <c r="B203" t="n">
-        <v>0.004115263345222564</v>
+        <v>0.003131004120381159</v>
       </c>
       <c r="C203" t="n">
-        <v>0.5131228642490717</v>
+        <v>0.5122323292129521</v>
       </c>
       <c r="D203" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>1010</v>
+        <v>2760</v>
       </c>
       <c r="B204" t="n">
-        <v>0.004057703902103684</v>
+        <v>0.003124092627403034</v>
       </c>
       <c r="C204" t="n">
-        <v>0.5131804236921906</v>
+        <v>0.5122392407059303</v>
       </c>
       <c r="D204" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>1015</v>
+        <v>2820</v>
       </c>
       <c r="B205" t="n">
-        <v>0.003955046559571385</v>
+        <v>0.003070131430221669</v>
       </c>
       <c r="C205" t="n">
-        <v>0.513283081034723</v>
+        <v>0.5122932019031116</v>
       </c>
       <c r="D205" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>1020</v>
+        <v>2880</v>
       </c>
       <c r="B206" t="n">
-        <v>0.003874612987789214</v>
+        <v>0.003075300787604444</v>
       </c>
       <c r="C206" t="n">
-        <v>0.5133635146065051</v>
+        <v>0.5122880325457289</v>
       </c>
       <c r="D206" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>1025</v>
-      </c>
-      <c r="B207" t="n">
-        <v>0.003877267763313047</v>
-      </c>
-      <c r="C207" t="n">
-        <v>0.5133608598309812</v>
-      </c>
-      <c r="D207" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>1030</v>
-      </c>
-      <c r="B208" t="n">
-        <v>0.00399536712455865</v>
-      </c>
-      <c r="C208" t="n">
-        <v>0.5132427604697357</v>
-      </c>
-      <c r="D208" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>1035</v>
-      </c>
-      <c r="B209" t="n">
-        <v>0.003798760201731391</v>
-      </c>
-      <c r="C209" t="n">
-        <v>0.5134393673925629</v>
-      </c>
-      <c r="D209" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="n">
-        <v>1040</v>
-      </c>
-      <c r="B210" t="n">
-        <v>0.003817250056175437</v>
-      </c>
-      <c r="C210" t="n">
-        <v>0.5134208775381189</v>
-      </c>
-      <c r="D210" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="n">
-        <v>1045</v>
-      </c>
-      <c r="B211" t="n">
-        <v>0.003822534739517828</v>
-      </c>
-      <c r="C211" t="n">
-        <v>0.5134155928547764</v>
-      </c>
-      <c r="D211" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>1050</v>
-      </c>
-      <c r="B212" t="n">
-        <v>0.003865718694940295</v>
-      </c>
-      <c r="C212" t="n">
-        <v>0.513372408899354</v>
-      </c>
-      <c r="D212" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>1055</v>
-      </c>
-      <c r="B213" t="n">
-        <v>0.003751248659390751</v>
-      </c>
-      <c r="C213" t="n">
-        <v>0.5134868789349035</v>
-      </c>
-      <c r="D213" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="n">
-        <v>1060</v>
-      </c>
-      <c r="B214" t="n">
-        <v>0.00374116477433554</v>
-      </c>
-      <c r="C214" t="n">
-        <v>0.5134969628199588</v>
-      </c>
-      <c r="D214" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="n">
-        <v>1065</v>
-      </c>
-      <c r="B215" t="n">
-        <v>0.003747889926739727</v>
-      </c>
-      <c r="C215" t="n">
-        <v>0.5134902376675546</v>
-      </c>
-      <c r="D215" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="n">
-        <v>1070</v>
-      </c>
-      <c r="B216" t="n">
-        <v>0.003924884411821149</v>
-      </c>
-      <c r="C216" t="n">
-        <v>0.5133132431824732</v>
-      </c>
-      <c r="D216" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>1075</v>
-      </c>
-      <c r="B217" t="n">
-        <v>0.003960793943134586</v>
-      </c>
-      <c r="C217" t="n">
-        <v>0.5132773336511598</v>
-      </c>
-      <c r="D217" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="n">
-        <v>1080</v>
-      </c>
-      <c r="B218" t="n">
-        <v>0.004018604929488546</v>
-      </c>
-      <c r="C218" t="n">
-        <v>0.5132195226648057</v>
-      </c>
-      <c r="D218" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>1085</v>
-      </c>
-      <c r="B219" t="n">
-        <v>0.003941831288961132</v>
-      </c>
-      <c r="C219" t="n">
-        <v>0.5132962963053332</v>
-      </c>
-      <c r="D219" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>1090</v>
-      </c>
-      <c r="B220" t="n">
-        <v>0.003943236479205818</v>
-      </c>
-      <c r="C220" t="n">
-        <v>0.5132948911150885</v>
-      </c>
-      <c r="D220" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>1095</v>
-      </c>
-      <c r="B221" t="n">
-        <v>0.004130188093298078</v>
-      </c>
-      <c r="C221" t="n">
-        <v>0.5131079395009962</v>
-      </c>
-      <c r="D221" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>1100</v>
-      </c>
-      <c r="B222" t="n">
-        <v>0.004227427288297052</v>
-      </c>
-      <c r="C222" t="n">
-        <v>0.5130107003059973</v>
-      </c>
-      <c r="D222" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>1105</v>
-      </c>
-      <c r="B223" t="n">
-        <v>0.004194599509979719</v>
-      </c>
-      <c r="C223" t="n">
-        <v>0.5130435280843146</v>
-      </c>
-      <c r="D223" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="n">
-        <v>1110</v>
-      </c>
-      <c r="B224" t="n">
-        <v>0.004168635604123404</v>
-      </c>
-      <c r="C224" t="n">
-        <v>0.5130694919901709</v>
-      </c>
-      <c r="D224" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="n">
-        <v>1115</v>
-      </c>
-      <c r="B225" t="n">
-        <v>0.004260239334588381</v>
-      </c>
-      <c r="C225" t="n">
-        <v>0.5129778882597059</v>
-      </c>
-      <c r="D225" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="n">
-        <v>1120</v>
-      </c>
-      <c r="B226" t="n">
-        <v>0.004316533290212638</v>
-      </c>
-      <c r="C226" t="n">
-        <v>0.5129215943040817</v>
-      </c>
-      <c r="D226" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="n">
-        <v>1125</v>
-      </c>
-      <c r="B227" t="n">
-        <v>0.004171087450609863</v>
-      </c>
-      <c r="C227" t="n">
-        <v>0.5130670401436844</v>
-      </c>
-      <c r="D227" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="n">
-        <v>1130</v>
-      </c>
-      <c r="B228" t="n">
-        <v>0.004109841104897223</v>
-      </c>
-      <c r="C228" t="n">
-        <v>0.5131282864893971</v>
-      </c>
-      <c r="D228" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="n">
-        <v>1135</v>
-      </c>
-      <c r="B229" t="n">
-        <v>0.004266247807350756</v>
-      </c>
-      <c r="C229" t="n">
-        <v>0.5129718797869436</v>
-      </c>
-      <c r="D229" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="n">
-        <v>1140</v>
-      </c>
-      <c r="B230" t="n">
-        <v>0.00395431916956172</v>
-      </c>
-      <c r="C230" t="n">
-        <v>0.5132838084247326</v>
-      </c>
-      <c r="D230" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="n">
-        <v>1145</v>
-      </c>
-      <c r="B231" t="n">
-        <v>0.004007883523124275</v>
-      </c>
-      <c r="C231" t="n">
-        <v>0.51323024407117</v>
-      </c>
-      <c r="D231" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="n">
-        <v>1150</v>
-      </c>
-      <c r="B232" t="n">
-        <v>0.003906863915536307</v>
-      </c>
-      <c r="C232" t="n">
-        <v>0.513331263678758</v>
-      </c>
-      <c r="D232" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="n">
-        <v>1155</v>
-      </c>
-      <c r="B233" t="n">
-        <v>0.003748272825541379</v>
-      </c>
-      <c r="C233" t="n">
-        <v>0.513489854768753</v>
-      </c>
-      <c r="D233" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="n">
-        <v>1160</v>
-      </c>
-      <c r="B234" t="n">
-        <v>0.003964578680049407</v>
-      </c>
-      <c r="C234" t="n">
-        <v>0.5132735489142449</v>
-      </c>
-      <c r="D234" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="n">
-        <v>1165</v>
-      </c>
-      <c r="B235" t="n">
-        <v>0.003817800691740445</v>
-      </c>
-      <c r="C235" t="n">
-        <v>0.5134203269025539</v>
-      </c>
-      <c r="D235" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="n">
-        <v>1170</v>
-      </c>
-      <c r="B236" t="n">
-        <v>0.003791331386147595</v>
-      </c>
-      <c r="C236" t="n">
-        <v>0.5134467962081467</v>
-      </c>
-      <c r="D236" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="n">
-        <v>1175</v>
-      </c>
-      <c r="B237" t="n">
-        <v>0.003736678926964537</v>
-      </c>
-      <c r="C237" t="n">
-        <v>0.5135014486673298</v>
-      </c>
-      <c r="D237" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="n">
-        <v>1180</v>
-      </c>
-      <c r="B238" t="n">
-        <v>0.003451243741487863</v>
-      </c>
-      <c r="C238" t="n">
-        <v>0.5137868838528065</v>
-      </c>
-      <c r="D238" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="n">
-        <v>1185</v>
-      </c>
-      <c r="B239" t="n">
-        <v>0.003441953637176138</v>
-      </c>
-      <c r="C239" t="n">
-        <v>0.5137961739571182</v>
-      </c>
-      <c r="D239" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="n">
-        <v>1190</v>
-      </c>
-      <c r="B240" t="n">
-        <v>0.003374848825735578</v>
-      </c>
-      <c r="C240" t="n">
-        <v>0.5138632787685588</v>
-      </c>
-      <c r="D240" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="n">
-        <v>1195</v>
-      </c>
-      <c r="B241" t="n">
-        <v>0.003498985519715809</v>
-      </c>
-      <c r="C241" t="n">
-        <v>0.5137391420745785</v>
-      </c>
-      <c r="D241" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="n">
-        <v>1200</v>
-      </c>
-      <c r="B242" t="n">
-        <v>0.003299977376527945</v>
-      </c>
-      <c r="C242" t="n">
-        <v>0.5139381502177663</v>
-      </c>
-      <c r="D242" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="n">
-        <v>1205</v>
-      </c>
-      <c r="B243" t="n">
-        <v>0.00324083163024218</v>
-      </c>
-      <c r="C243" t="n">
-        <v>0.5139972959640522</v>
-      </c>
-      <c r="D243" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="n">
-        <v>1210</v>
-      </c>
-      <c r="B244" t="n">
-        <v>0.00352334070358461</v>
-      </c>
-      <c r="C244" t="n">
-        <v>0.5137147868907097</v>
-      </c>
-      <c r="D244" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="n">
-        <v>1215</v>
-      </c>
-      <c r="B245" t="n">
-        <v>0.003390049313364528</v>
-      </c>
-      <c r="C245" t="n">
-        <v>0.5138480782809298</v>
-      </c>
-      <c r="D245" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="n">
-        <v>1220</v>
-      </c>
-      <c r="B246" t="n">
-        <v>0.003266150048352392</v>
-      </c>
-      <c r="C246" t="n">
-        <v>0.5139719775459419</v>
-      </c>
-      <c r="D246" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="n">
-        <v>1225</v>
-      </c>
-      <c r="B247" t="n">
-        <v>0.003288362381381049</v>
-      </c>
-      <c r="C247" t="n">
-        <v>0.5139497652129132</v>
-      </c>
-      <c r="D247" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>1230</v>
-      </c>
-      <c r="B248" t="n">
-        <v>0.003129810854307797</v>
-      </c>
-      <c r="C248" t="n">
-        <v>0.5141083167399866</v>
-      </c>
-      <c r="D248" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>1235</v>
-      </c>
-      <c r="B249" t="n">
-        <v>0.003169800244078439</v>
-      </c>
-      <c r="C249" t="n">
-        <v>0.5140683273502159</v>
-      </c>
-      <c r="D249" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>1240</v>
-      </c>
-      <c r="B250" t="n">
-        <v>0.003088410865399451</v>
-      </c>
-      <c r="C250" t="n">
-        <v>0.5141497167288949</v>
-      </c>
-      <c r="D250" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>1245</v>
-      </c>
-      <c r="B251" t="n">
-        <v>0.003109566458209632</v>
-      </c>
-      <c r="C251" t="n">
-        <v>0.5141285611360847</v>
-      </c>
-      <c r="D251" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="n">
-        <v>1250</v>
-      </c>
-      <c r="B252" t="n">
-        <v>0.002886752511842268</v>
-      </c>
-      <c r="C252" t="n">
-        <v>0.5143513750824521</v>
-      </c>
-      <c r="D252" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="n">
-        <v>1255</v>
-      </c>
-      <c r="B253" t="n">
-        <v>0.002920352138861053</v>
-      </c>
-      <c r="C253" t="n">
-        <v>0.5143177754554332</v>
-      </c>
-      <c r="D253" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="n">
-        <v>1260</v>
-      </c>
-      <c r="B254" t="n">
-        <v>0.002999236177549103</v>
-      </c>
-      <c r="C254" t="n">
-        <v>0.5142388914167452</v>
-      </c>
-      <c r="D254" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="n">
-        <v>1265</v>
-      </c>
-      <c r="B255" t="n">
-        <v>0.002931539817402583</v>
-      </c>
-      <c r="C255" t="n">
-        <v>0.5143065877768918</v>
-      </c>
-      <c r="D255" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="n">
-        <v>1270</v>
-      </c>
-      <c r="B256" t="n">
-        <v>0.002889437228891886</v>
-      </c>
-      <c r="C256" t="n">
-        <v>0.5143486903654024</v>
-      </c>
-      <c r="D256" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="n">
-        <v>1275</v>
-      </c>
-      <c r="B257" t="n">
-        <v>0.002926694776062454</v>
-      </c>
-      <c r="C257" t="n">
-        <v>0.5143114328182319</v>
-      </c>
-      <c r="D257" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="n">
-        <v>1280</v>
-      </c>
-      <c r="B258" t="n">
-        <v>0.00285618836961568</v>
-      </c>
-      <c r="C258" t="n">
-        <v>0.5143819392246787</v>
-      </c>
-      <c r="D258" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="n">
-        <v>1285</v>
-      </c>
-      <c r="B259" t="n">
-        <v>0.002930255446441583</v>
-      </c>
-      <c r="C259" t="n">
-        <v>0.5143078721478528</v>
-      </c>
-      <c r="D259" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="n">
-        <v>1290</v>
-      </c>
-      <c r="B260" t="n">
-        <v>0.002879328975370913</v>
-      </c>
-      <c r="C260" t="n">
-        <v>0.5143587986189234</v>
-      </c>
-      <c r="D260" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="n">
-        <v>1295</v>
-      </c>
-      <c r="B261" t="n">
-        <v>0.002937633719207312</v>
-      </c>
-      <c r="C261" t="n">
-        <v>0.514300493875087</v>
-      </c>
-      <c r="D261" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="n">
-        <v>1300</v>
-      </c>
-      <c r="B262" t="n">
-        <v>0.002883650008467203</v>
-      </c>
-      <c r="C262" t="n">
-        <v>0.5143544775858271</v>
-      </c>
-      <c r="D262" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="n">
-        <v>1305</v>
-      </c>
-      <c r="B263" t="n">
-        <v>0.002877767790897015</v>
-      </c>
-      <c r="C263" t="n">
-        <v>0.5143603598033973</v>
-      </c>
-      <c r="D263" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="n">
-        <v>1310</v>
-      </c>
-      <c r="B264" t="n">
-        <v>0.002873519328879188</v>
-      </c>
-      <c r="C264" t="n">
-        <v>0.5143646082654152</v>
-      </c>
-      <c r="D264" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="n">
-        <v>1315</v>
-      </c>
-      <c r="B265" t="n">
-        <v>0.003116645446479973</v>
-      </c>
-      <c r="C265" t="n">
-        <v>0.5141214821478144</v>
-      </c>
-      <c r="D265" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="n">
-        <v>1320</v>
-      </c>
-      <c r="B266" t="n">
-        <v>0.002896137206788638</v>
-      </c>
-      <c r="C266" t="n">
-        <v>0.5143419903875057</v>
-      </c>
-      <c r="D266" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="n">
-        <v>1325</v>
-      </c>
-      <c r="B267" t="n">
-        <v>0.003123767043463381</v>
-      </c>
-      <c r="C267" t="n">
-        <v>0.5141143605508309</v>
-      </c>
-      <c r="D267" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="n">
-        <v>1330</v>
-      </c>
-      <c r="B268" t="n">
-        <v>0.002906693028788932</v>
-      </c>
-      <c r="C268" t="n">
-        <v>0.5143314345655053</v>
-      </c>
-      <c r="D268" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="n">
-        <v>1335</v>
-      </c>
-      <c r="B269" t="n">
-        <v>0.003147773611939959</v>
-      </c>
-      <c r="C269" t="n">
-        <v>0.5140903539823544</v>
-      </c>
-      <c r="D269" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="n">
-        <v>1340</v>
-      </c>
-      <c r="B270" t="n">
-        <v>0.002870263048454402</v>
-      </c>
-      <c r="C270" t="n">
-        <v>0.5143678645458399</v>
-      </c>
-      <c r="D270" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="n">
-        <v>1345</v>
-      </c>
-      <c r="B271" t="n">
-        <v>0.003102678417415275</v>
-      </c>
-      <c r="C271" t="n">
-        <v>0.514135449176879</v>
-      </c>
-      <c r="D271" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="n">
-        <v>1350</v>
-      </c>
-      <c r="B272" t="n">
-        <v>0.002898944891879994</v>
-      </c>
-      <c r="C272" t="n">
-        <v>0.5143391827024143</v>
-      </c>
-      <c r="D272" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="n">
-        <v>1355</v>
-      </c>
-      <c r="B273" t="n">
-        <v>0.003099584159442789</v>
-      </c>
-      <c r="C273" t="n">
-        <v>0.5141385434348515</v>
-      </c>
-      <c r="D273" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="n">
-        <v>1360</v>
-      </c>
-      <c r="B274" t="n">
-        <v>0.003075554311733155</v>
-      </c>
-      <c r="C274" t="n">
-        <v>0.5141625732825612</v>
-      </c>
-      <c r="D274" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="n">
-        <v>1365</v>
-      </c>
-      <c r="B275" t="n">
-        <v>0.002979921986466589</v>
-      </c>
-      <c r="C275" t="n">
-        <v>0.5142582056078278</v>
-      </c>
-      <c r="D275" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="n">
-        <v>1370</v>
-      </c>
-      <c r="B276" t="n">
-        <v>0.002918059454387303</v>
-      </c>
-      <c r="C276" t="n">
-        <v>0.514320068139907</v>
-      </c>
-      <c r="D276" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="n">
-        <v>1375</v>
-      </c>
-      <c r="B277" t="n">
-        <v>0.002974425780333106</v>
-      </c>
-      <c r="C277" t="n">
-        <v>0.5142637018139612</v>
-      </c>
-      <c r="D277" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="n">
-        <v>1380</v>
-      </c>
-      <c r="B278" t="n">
-        <v>0.00294898443510093</v>
-      </c>
-      <c r="C278" t="n">
-        <v>0.5142891431591934</v>
-      </c>
-      <c r="D278" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="n">
-        <v>1385</v>
-      </c>
-      <c r="B279" t="n">
-        <v>0.002809659426696972</v>
-      </c>
-      <c r="C279" t="n">
-        <v>0.5144284681675974</v>
-      </c>
-      <c r="D279" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="n">
-        <v>1390</v>
-      </c>
-      <c r="B280" t="n">
-        <v>0.002886874883695162</v>
-      </c>
-      <c r="C280" t="n">
-        <v>0.5143512527105991</v>
-      </c>
-      <c r="D280" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="n">
-        <v>1395</v>
-      </c>
-      <c r="B281" t="n">
-        <v>0.002882983700173221</v>
-      </c>
-      <c r="C281" t="n">
-        <v>0.5143551438941211</v>
-      </c>
-      <c r="D281" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="n">
-        <v>1400</v>
-      </c>
-      <c r="B282" t="n">
-        <v>0.002887746383944999</v>
-      </c>
-      <c r="C282" t="n">
-        <v>0.5143503812103494</v>
-      </c>
-      <c r="D282" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="n">
-        <v>1405</v>
-      </c>
-      <c r="B283" t="n">
-        <v>0.002877536594070744</v>
-      </c>
-      <c r="C283" t="n">
-        <v>0.5143605910002236</v>
-      </c>
-      <c r="D283" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="n">
-        <v>1410</v>
-      </c>
-      <c r="B284" t="n">
-        <v>0.002882426639827119</v>
-      </c>
-      <c r="C284" t="n">
-        <v>0.5143557009544673</v>
-      </c>
-      <c r="D284" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="n">
-        <v>1415</v>
-      </c>
-      <c r="B285" t="n">
-        <v>0.002800850206642337</v>
-      </c>
-      <c r="C285" t="n">
-        <v>0.514437277387652</v>
-      </c>
-      <c r="D285" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="n">
-        <v>1420</v>
-      </c>
-      <c r="B286" t="n">
-        <v>0.002796658378209698</v>
-      </c>
-      <c r="C286" t="n">
-        <v>0.5144414692160846</v>
-      </c>
-      <c r="D286" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="n">
-        <v>1425</v>
-      </c>
-      <c r="B287" t="n">
-        <v>0.002791123770539555</v>
-      </c>
-      <c r="C287" t="n">
-        <v>0.5144470038237547</v>
-      </c>
-      <c r="D287" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="n">
-        <v>1430</v>
-      </c>
-      <c r="B288" t="n">
-        <v>0.00276670347535892</v>
-      </c>
-      <c r="C288" t="n">
-        <v>0.5144714241189354</v>
-      </c>
-      <c r="D288" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="n">
-        <v>1435</v>
-      </c>
-      <c r="B289" t="n">
-        <v>0.00281392557080922</v>
-      </c>
-      <c r="C289" t="n">
-        <v>0.5144242020234852</v>
-      </c>
-      <c r="D289" t="n">
-        <v>0.5172381275942943</v>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="n">
-        <v>1440</v>
-      </c>
-      <c r="B290" t="n">
-        <v>0.002231824988326103</v>
-      </c>
-      <c r="C290" t="n">
-        <v>0.5150063026059682</v>
-      </c>
-      <c r="D290" t="n">
-        <v>0.5172381275942943</v>
+        <v>0.5153633333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>